<commit_message>
added a revenue source to the file that appeared in 2018 and never had a revenue type. Now rev_NA no longer exist because all revenue items have a rev_type code in FY23 data!
</commit_message>
<xml_diff>
--- a/data/ioc_source_updated23_AWM.xlsx
+++ b/data/ioc_source_updated23_AWM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleaw\OneDrive\Documents\PhD Fall 2021 - Spring 2022\Merriman RA\Fiscal Futures IGPA\Fiscal Futures FY2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleaw\OneDrive\Documents\PhD Fall 2021 - Spring 2022\Merriman RA\Fiscal Futures IGPA\Fiscal Futures FY2023\Fiscal-Future-Topics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2B251D-8926-4606-BED4-D66483BBE2CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D9A5A4-07D5-45A8-B59A-09C14D26A483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8640" yWindow="0" windowWidth="14400" windowHeight="12960" xr2:uid="{95DD0F56-1BF5-4636-A2E6-971DE42DAC47}"/>
+    <workbookView xWindow="-14400" yWindow="5550" windowWidth="14400" windowHeight="15600" xr2:uid="{95DD0F56-1BF5-4636-A2E6-971DE42DAC47}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="14" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12350" uniqueCount="4851">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12355" uniqueCount="4853">
   <si>
     <t>source</t>
   </si>
@@ -14590,6 +14590,12 @@
   </si>
   <si>
     <t>FED MONIES VIA IDVA</t>
+  </si>
+  <si>
+    <t>2607</t>
+  </si>
+  <si>
+    <t>PRIVATE ORG OR INDI/SHEEO</t>
   </si>
 </sst>
 </file>
@@ -15045,7 +15051,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{49EEBAE8-29F6-463B-9B2F-33AF9E80ABD6}" name="PivotTable2" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{49EEBAE8-29F6-463B-9B2F-33AF9E80ABD6}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="J1:K41" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" outline="0" showAll="0" defaultSubtotal="0">
@@ -15319,8 +15325,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{35C46ACB-F213-49A5-9C6B-6F57AA7FB6BB}" name="Table2" displayName="Table2" ref="A1:H2425" totalsRowShown="0">
-  <autoFilter ref="A1:H2425" xr:uid="{35C46ACB-F213-49A5-9C6B-6F57AA7FB6BB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{35C46ACB-F213-49A5-9C6B-6F57AA7FB6BB}" name="Table2" displayName="Table2" ref="A1:H2426" totalsRowShown="0">
+  <autoFilter ref="A1:H2426" xr:uid="{35C46ACB-F213-49A5-9C6B-6F57AA7FB6BB}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H2425">
     <sortCondition ref="C1:C2425"/>
   </sortState>
@@ -15649,10 +15655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L2425"/>
+  <dimension ref="A1:L2426"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="B2357" workbookViewId="0">
+      <selection activeCell="H2427" sqref="H2427"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -58030,6 +58036,23 @@
       </c>
       <c r="H2425" t="s">
         <v>4816</v>
+      </c>
+    </row>
+    <row r="2426" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2426" s="7" t="s">
+        <v>4851</v>
+      </c>
+      <c r="B2426" t="s">
+        <v>4852</v>
+      </c>
+      <c r="C2426" s="7" t="s">
+        <v>4747</v>
+      </c>
+      <c r="D2426" t="s">
+        <v>4801</v>
+      </c>
+      <c r="H2426" t="s">
+        <v>4810</v>
       </c>
     </row>
   </sheetData>

</xml_diff>